<commit_message>
Add experiment results for 5 fold CVs with more records resulted from filtering based on 3 features
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/Bank_Classification_Results_using_5_fold_CV.xlsx
+++ b/Experiment_Resulsts/Bank_Classification_Results_using_5_fold_CV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_mces_bank_data\Experiment_Resulsts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0658B4E2-5478-4E0F-8CD8-FD217513457C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AF754B-3980-4384-B779-7959E76C0704}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{98666712-FD92-4C48-8ABF-24F5869146C3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="27">
   <si>
     <t>Last Record</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>5 Features</t>
+  </si>
+  <si>
+    <t>More Records</t>
+  </si>
+  <si>
+    <t>Now</t>
+  </si>
+  <si>
+    <t>Previous</t>
   </si>
 </sst>
 </file>
@@ -211,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,6 +238,11 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DCF0E0-FAAB-441A-A370-B138D481EADA}">
-  <dimension ref="A1:W30"/>
+  <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,7 +618,16 @@
         <v>0</v>
       </c>
       <c r="H2" s="13"/>
+      <c r="I2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>3105</v>
+      </c>
       <c r="P2" s="13"/>
+      <c r="Q2" s="6" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -1062,6 +1085,9 @@
       <c r="I12" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="K12" s="3">
+        <v>3048</v>
+      </c>
       <c r="P12" s="13"/>
       <c r="Q12" s="3" t="s">
         <v>13</v>
@@ -1523,6 +1549,9 @@
       <c r="I22" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="K22" s="8">
+        <v>2945</v>
+      </c>
       <c r="P22" s="13"/>
       <c r="Q22" s="8" t="s">
         <v>14</v>
@@ -1971,6 +2000,622 @@
         <v>0</v>
       </c>
       <c r="W30" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="K33" t="s">
+        <v>25</v>
+      </c>
+      <c r="L33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I34" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K34" s="15">
+        <v>3549</v>
+      </c>
+      <c r="L34" s="16">
+        <v>3105</v>
+      </c>
+      <c r="M34" s="19">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="35" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+    </row>
+    <row r="36" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="J36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I37" t="s">
+        <v>5</v>
+      </c>
+      <c r="J37">
+        <v>0.38685463349703503</v>
+      </c>
+      <c r="K37">
+        <v>3.3846424797463901</v>
+      </c>
+      <c r="L37">
+        <v>0.33820954422606297</v>
+      </c>
+      <c r="M37">
+        <v>84.671738517892393</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37"/>
+    </row>
+    <row r="38" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I38" t="s">
+        <v>6</v>
+      </c>
+      <c r="J38">
+        <v>0.38527866631986701</v>
+      </c>
+      <c r="K38">
+        <v>3.2113420218386799</v>
+      </c>
+      <c r="L38">
+        <v>0.34110516765419902</v>
+      </c>
+      <c r="M38">
+        <v>84.847844463229094</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38"/>
+    </row>
+    <row r="39" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J39">
+        <v>0.381809211261667</v>
+      </c>
+      <c r="K39">
+        <v>3.3282846072560801</v>
+      </c>
+      <c r="L39">
+        <v>0.35937604856691402</v>
+      </c>
+      <c r="M39">
+        <v>85.059171597633096</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39"/>
+    </row>
+    <row r="40" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I40" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40">
+        <v>0.38877908208885698</v>
+      </c>
+      <c r="K40">
+        <v>3.2617118703768901</v>
+      </c>
+      <c r="L40">
+        <v>0.32211374243934798</v>
+      </c>
+      <c r="M40">
+        <v>84.249084249084305</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40"/>
+    </row>
+    <row r="41" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I41" t="s">
+        <v>9</v>
+      </c>
+      <c r="J41">
+        <v>0.388386430803427</v>
+      </c>
+      <c r="K41">
+        <v>3.4251497005988001</v>
+      </c>
+      <c r="L41">
+        <v>0.32841923761511999</v>
+      </c>
+      <c r="M41">
+        <v>84.601296139757693</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41"/>
+    </row>
+    <row r="43" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J43" s="2">
+        <v>0.386221604794171</v>
+      </c>
+      <c r="K43" s="2">
+        <v>3.3222261359633598</v>
+      </c>
+      <c r="L43" s="2">
+        <v>0.337844748100329</v>
+      </c>
+      <c r="M43" s="5">
+        <v>84.685826993519299</v>
+      </c>
+      <c r="N43" s="2">
+        <v>0</v>
+      </c>
+      <c r="O43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+    </row>
+    <row r="45" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" t="s">
+        <v>25</v>
+      </c>
+      <c r="L45" t="s">
+        <v>26</v>
+      </c>
+      <c r="M45" s="5"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+    </row>
+    <row r="46" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I46" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K46" s="15">
+        <v>3486</v>
+      </c>
+      <c r="L46" s="17">
+        <v>3048</v>
+      </c>
+      <c r="M46" s="19">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="47" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I47" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+    </row>
+    <row r="48" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="J48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I49" t="s">
+        <v>5</v>
+      </c>
+      <c r="J49">
+        <v>0.40355054563062798</v>
+      </c>
+      <c r="K49">
+        <v>3.9479913916786198</v>
+      </c>
+      <c r="L49">
+        <v>0.16900374856188899</v>
+      </c>
+      <c r="M49">
+        <v>85.233792312105606</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49"/>
+    </row>
+    <row r="50" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I50" t="s">
+        <v>6</v>
+      </c>
+      <c r="J50">
+        <v>0.39234229021313999</v>
+      </c>
+      <c r="K50">
+        <v>4.1119081779053097</v>
+      </c>
+      <c r="L50">
+        <v>0.21271016588104399</v>
+      </c>
+      <c r="M50">
+        <v>84.731784279977106</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50"/>
+    </row>
+    <row r="51" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I51" t="s">
+        <v>7</v>
+      </c>
+      <c r="J51">
+        <v>0.39716847615026901</v>
+      </c>
+      <c r="K51">
+        <v>3.8719512195122001</v>
+      </c>
+      <c r="L51">
+        <v>0.20810523489723601</v>
+      </c>
+      <c r="M51">
+        <v>84.301491681009793</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51"/>
+    </row>
+    <row r="52" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I52" t="s">
+        <v>8</v>
+      </c>
+      <c r="J52">
+        <v>0.41185298599478498</v>
+      </c>
+      <c r="K52">
+        <v>3.8576040172166399</v>
+      </c>
+      <c r="L52">
+        <v>0.13350501849801699</v>
+      </c>
+      <c r="M52">
+        <v>84.624211130235196</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="P52"/>
+    </row>
+    <row r="53" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I53" t="s">
+        <v>9</v>
+      </c>
+      <c r="J53">
+        <v>0.39534614762758002</v>
+      </c>
+      <c r="K53">
+        <v>3.5053802008608299</v>
+      </c>
+      <c r="L53">
+        <v>0.22419995818811</v>
+      </c>
+      <c r="M53">
+        <v>84.158060814687303</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53"/>
+    </row>
+    <row r="55" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J55" s="2">
+        <v>0.400052089123281</v>
+      </c>
+      <c r="K55" s="2">
+        <v>3.8589670014347202</v>
+      </c>
+      <c r="L55" s="2">
+        <v>0.18950482520525899</v>
+      </c>
+      <c r="M55" s="5">
+        <v>84.609868043602901</v>
+      </c>
+      <c r="N55" s="2">
+        <v>0</v>
+      </c>
+      <c r="O55" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+    </row>
+    <row r="57" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" t="s">
+        <v>25</v>
+      </c>
+      <c r="L57" t="s">
+        <v>26</v>
+      </c>
+      <c r="M57" s="5"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+    </row>
+    <row r="58" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I58" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K58" s="15">
+        <v>3404</v>
+      </c>
+      <c r="L58" s="18">
+        <v>2945</v>
+      </c>
+      <c r="M58" s="19">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="59" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I59" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
+      <c r="O59" s="9"/>
+    </row>
+    <row r="60" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="J60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I61" t="s">
+        <v>5</v>
+      </c>
+      <c r="J61">
+        <v>0.37339605760431099</v>
+      </c>
+      <c r="K61">
+        <v>4.3532868160117504</v>
+      </c>
+      <c r="L61">
+        <v>0.190222077894903</v>
+      </c>
+      <c r="M61">
+        <v>85.744712103407807</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="P61"/>
+    </row>
+    <row r="62" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I62" t="s">
+        <v>6</v>
+      </c>
+      <c r="J62">
+        <v>0.37370172629599102</v>
+      </c>
+      <c r="K62">
+        <v>4.2757987513771596</v>
+      </c>
+      <c r="L62">
+        <v>0.195583350481667</v>
+      </c>
+      <c r="M62">
+        <v>85.634547591069307</v>
+      </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="P62"/>
+    </row>
+    <row r="63" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I63" t="s">
+        <v>7</v>
+      </c>
+      <c r="J63">
+        <v>0.375563559008249</v>
+      </c>
+      <c r="K63">
+        <v>4.7172236503856002</v>
+      </c>
+      <c r="L63">
+        <v>0.19151985001373001</v>
+      </c>
+      <c r="M63">
+        <v>85.487661574618102</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63"/>
+    </row>
+    <row r="64" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I64" t="s">
+        <v>8</v>
+      </c>
+      <c r="J64">
+        <v>0.37881359954251698</v>
+      </c>
+      <c r="K64">
+        <v>4.3731178846860104</v>
+      </c>
+      <c r="L64">
+        <v>0.14126264258670099</v>
+      </c>
+      <c r="M64">
+        <v>85.340775558166897</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="P64"/>
+    </row>
+    <row r="65" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I65" t="s">
+        <v>9</v>
+      </c>
+      <c r="J65">
+        <v>0.36382685234353201</v>
+      </c>
+      <c r="K65">
+        <v>4.4531766434080096</v>
+      </c>
+      <c r="L65">
+        <v>0.25322780262036299</v>
+      </c>
+      <c r="M65">
+        <v>86.479142185663903</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="P65"/>
+    </row>
+    <row r="67" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="I67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J67" s="2">
+        <v>0.37306035895891998</v>
+      </c>
+      <c r="K67" s="2">
+        <v>4.4345207491737</v>
+      </c>
+      <c r="L67" s="2">
+        <v>0.194363144719473</v>
+      </c>
+      <c r="M67" s="14">
+        <v>85.737367802585197</v>
+      </c>
+      <c r="N67" s="2">
+        <v>0</v>
+      </c>
+      <c r="O67" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update results for 5-fold cross valdiation classification using emfis with reconstructed data
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/Bank_Classification_Results_using_5_fold_CV.xlsx
+++ b/Experiment_Resulsts/Bank_Classification_Results_using_5_fold_CV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_mces_bank_data\Experiment_Resulsts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_predict_bank_failure\Experiment_Resulsts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AF754B-3980-4384-B779-7959E76C0704}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3178AB3A-51CE-4700-9A90-6A38258A7FA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{98666712-FD92-4C48-8ABF-24F5869146C3}"/>
+    <workbookView xWindow="60" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{98666712-FD92-4C48-8ABF-24F5869146C3}"/>
   </bookViews>
   <sheets>
     <sheet name="5_Fold" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="28">
   <si>
     <t>Last Record</t>
   </si>
@@ -113,12 +113,15 @@
   <si>
     <t>Previous</t>
   </si>
+  <si>
+    <t>After reconstruction</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +161,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -220,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -243,6 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DCF0E0-FAAB-441A-A370-B138D481EADA}">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z10" activeCellId="1" sqref="Z1 Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2003,15 +2015,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="9:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="9:23" ht="21" x14ac:dyDescent="0.4">
       <c r="K33" t="s">
         <v>25</v>
       </c>
       <c r="L33" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q33" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="S33" t="s">
+        <v>25</v>
+      </c>
+      <c r="T33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I34" s="15" t="s">
         <v>24</v>
       </c>
@@ -2024,8 +2045,20 @@
       <c r="M34" s="19">
         <v>444</v>
       </c>
-    </row>
-    <row r="35" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q34" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="S34" s="15">
+        <v>3636</v>
+      </c>
+      <c r="T34" s="16">
+        <v>3105</v>
+      </c>
+      <c r="U34" s="19">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="35" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I35" s="6" t="s">
         <v>0</v>
       </c>
@@ -2035,8 +2068,17 @@
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
-    </row>
-    <row r="36" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+    </row>
+    <row r="36" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J36" s="1" t="s">
         <v>1</v>
       </c>
@@ -2055,8 +2097,26 @@
       <c r="O36" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="R36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I37" t="s">
         <v>5</v>
       </c>
@@ -2079,8 +2139,29 @@
         <v>0</v>
       </c>
       <c r="P37"/>
-    </row>
-    <row r="38" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q37" t="s">
+        <v>5</v>
+      </c>
+      <c r="R37">
+        <v>0.42468834467962902</v>
+      </c>
+      <c r="S37">
+        <v>2.90680880330124</v>
+      </c>
+      <c r="T37">
+        <v>0.24936021443773501</v>
+      </c>
+      <c r="U37">
+        <v>82.4738723872387</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I38" t="s">
         <v>6</v>
       </c>
@@ -2103,8 +2184,29 @@
         <v>0</v>
       </c>
       <c r="P38"/>
-    </row>
-    <row r="39" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q38" t="s">
+        <v>6</v>
+      </c>
+      <c r="R38">
+        <v>0.43391842403958197</v>
+      </c>
+      <c r="S38">
+        <v>2.9604539202200799</v>
+      </c>
+      <c r="T38">
+        <v>0.200011912589205</v>
+      </c>
+      <c r="U38">
+        <v>82.714521452145206</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I39" t="s">
         <v>7</v>
       </c>
@@ -2127,8 +2229,29 @@
         <v>0</v>
       </c>
       <c r="P39"/>
-    </row>
-    <row r="40" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q39" t="s">
+        <v>7</v>
+      </c>
+      <c r="R39">
+        <v>0.42481404432117897</v>
+      </c>
+      <c r="S39">
+        <v>2.9343191196698801</v>
+      </c>
+      <c r="T39">
+        <v>0.244951255526521</v>
+      </c>
+      <c r="U39">
+        <v>82.680143014301393</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I40" t="s">
         <v>8</v>
       </c>
@@ -2151,8 +2274,29 @@
         <v>0</v>
       </c>
       <c r="P40"/>
-    </row>
-    <row r="41" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q40" t="s">
+        <v>8</v>
+      </c>
+      <c r="R40">
+        <v>0.43289219998512402</v>
+      </c>
+      <c r="S40">
+        <v>3.0072214580467702</v>
+      </c>
+      <c r="T40">
+        <v>0.229074346325643</v>
+      </c>
+      <c r="U40">
+        <v>82.095709570957098</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I41" t="s">
         <v>9</v>
       </c>
@@ -2175,8 +2319,29 @@
         <v>0</v>
       </c>
       <c r="P41"/>
-    </row>
-    <row r="43" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q41" t="s">
+        <v>9</v>
+      </c>
+      <c r="R41">
+        <v>0.42791777776504297</v>
+      </c>
+      <c r="S41">
+        <v>3.0154745529573601</v>
+      </c>
+      <c r="T41">
+        <v>0.229375078635878</v>
+      </c>
+      <c r="U41">
+        <v>83.264576457645802</v>
+      </c>
+      <c r="V41">
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I43" s="2" t="s">
         <v>10</v>
       </c>
@@ -2198,8 +2363,29 @@
       <c r="O43" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R43" s="2">
+        <v>0.428846158158111</v>
+      </c>
+      <c r="S43" s="2">
+        <v>2.96485557083906</v>
+      </c>
+      <c r="T43" s="2">
+        <v>0.230554561502997</v>
+      </c>
+      <c r="U43" s="14">
+        <v>82.645764576457594</v>
+      </c>
+      <c r="V43" s="2">
+        <v>0</v>
+      </c>
+      <c r="W43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
@@ -2207,8 +2393,15 @@
       <c r="M44" s="5"/>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
-    </row>
-    <row r="45" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+    </row>
+    <row r="45" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" t="s">
@@ -2220,8 +2413,19 @@
       <c r="M45" s="5"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
-    </row>
-    <row r="46" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" t="s">
+        <v>25</v>
+      </c>
+      <c r="T45" t="s">
+        <v>26</v>
+      </c>
+      <c r="U45" s="5"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+    </row>
+    <row r="46" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I46" s="15" t="s">
         <v>24</v>
       </c>
@@ -2234,8 +2438,20 @@
       <c r="M46" s="19">
         <v>438</v>
       </c>
-    </row>
-    <row r="47" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q46" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="S46" s="15">
+        <v>3624</v>
+      </c>
+      <c r="T46" s="17">
+        <v>3048</v>
+      </c>
+      <c r="U46" s="19">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="47" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I47" s="3" t="s">
         <v>13</v>
       </c>
@@ -2245,8 +2461,17 @@
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
-    </row>
-    <row r="48" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q47" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="4"/>
+    </row>
+    <row r="48" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J48" s="1" t="s">
         <v>1</v>
       </c>
@@ -2265,8 +2490,26 @@
       <c r="O48" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="R48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W48" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I49" t="s">
         <v>5</v>
       </c>
@@ -2289,8 +2532,29 @@
         <v>0</v>
       </c>
       <c r="P49"/>
-    </row>
-    <row r="50" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q49" t="s">
+        <v>5</v>
+      </c>
+      <c r="R49">
+        <v>0.422076357677725</v>
+      </c>
+      <c r="S49">
+        <v>3.7226629872369799</v>
+      </c>
+      <c r="T49">
+        <v>0.244556215563938</v>
+      </c>
+      <c r="U49">
+        <v>81.815673289183195</v>
+      </c>
+      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I50" t="s">
         <v>6</v>
       </c>
@@ -2313,8 +2577,29 @@
         <v>0</v>
       </c>
       <c r="P50"/>
-    </row>
-    <row r="51" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q50" t="s">
+        <v>6</v>
+      </c>
+      <c r="R50">
+        <v>0.43637081718394</v>
+      </c>
+      <c r="S50">
+        <v>3.2021386685063802</v>
+      </c>
+      <c r="T50">
+        <v>0.17632551169549501</v>
+      </c>
+      <c r="U50">
+        <v>80.470474613686505</v>
+      </c>
+      <c r="V50">
+        <v>0</v>
+      </c>
+      <c r="W50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I51" t="s">
         <v>7</v>
       </c>
@@ -2337,8 +2622,29 @@
         <v>0</v>
       </c>
       <c r="P51"/>
-    </row>
-    <row r="52" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q51" t="s">
+        <v>7</v>
+      </c>
+      <c r="R51">
+        <v>0.43170096363083499</v>
+      </c>
+      <c r="S51">
+        <v>3.3176957571576402</v>
+      </c>
+      <c r="T51">
+        <v>0.189766729623775</v>
+      </c>
+      <c r="U51">
+        <v>80.780905077262702</v>
+      </c>
+      <c r="V51">
+        <v>0</v>
+      </c>
+      <c r="W51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I52" t="s">
         <v>8</v>
       </c>
@@ -2361,8 +2667,29 @@
         <v>0</v>
       </c>
       <c r="P52"/>
-    </row>
-    <row r="53" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q52" t="s">
+        <v>8</v>
+      </c>
+      <c r="R52">
+        <v>0.42591862730208602</v>
+      </c>
+      <c r="S52">
+        <v>3.79199724042773</v>
+      </c>
+      <c r="T52">
+        <v>0.23846217680564999</v>
+      </c>
+      <c r="U52">
+        <v>81.160320088300196</v>
+      </c>
+      <c r="V52">
+        <v>0</v>
+      </c>
+      <c r="W52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I53" t="s">
         <v>9</v>
       </c>
@@ -2385,8 +2712,29 @@
         <v>0</v>
       </c>
       <c r="P53"/>
-    </row>
-    <row r="55" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q53" t="s">
+        <v>9</v>
+      </c>
+      <c r="R53">
+        <v>0.42076769168354</v>
+      </c>
+      <c r="S53">
+        <v>3.74611935150052</v>
+      </c>
+      <c r="T53">
+        <v>0.25384481380884699</v>
+      </c>
+      <c r="U53">
+        <v>81.6777041942605</v>
+      </c>
+      <c r="V53">
+        <v>0</v>
+      </c>
+      <c r="W53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I55" s="2" t="s">
         <v>10</v>
       </c>
@@ -2408,8 +2756,29 @@
       <c r="O55" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R55" s="2">
+        <v>0.42736689149562501</v>
+      </c>
+      <c r="S55" s="2">
+        <v>3.5561228009658499</v>
+      </c>
+      <c r="T55" s="2">
+        <v>0.22059108949954101</v>
+      </c>
+      <c r="U55" s="5">
+        <v>81.181015452538603</v>
+      </c>
+      <c r="V55" s="2">
+        <v>0</v>
+      </c>
+      <c r="W55" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
@@ -2417,8 +2786,15 @@
       <c r="M56" s="5"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
-    </row>
-    <row r="57" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+      <c r="U56" s="5"/>
+      <c r="V56" s="2"/>
+      <c r="W56" s="2"/>
+    </row>
+    <row r="57" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" t="s">
@@ -2430,8 +2806,19 @@
       <c r="M57" s="5"/>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
-    </row>
-    <row r="58" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
+      <c r="S57" t="s">
+        <v>25</v>
+      </c>
+      <c r="T57" t="s">
+        <v>26</v>
+      </c>
+      <c r="U57" s="5"/>
+      <c r="V57" s="2"/>
+      <c r="W57" s="2"/>
+    </row>
+    <row r="58" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I58" s="15" t="s">
         <v>24</v>
       </c>
@@ -2444,8 +2831,20 @@
       <c r="M58" s="19">
         <v>459</v>
       </c>
-    </row>
-    <row r="59" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q58" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="S58" s="15">
+        <v>3620</v>
+      </c>
+      <c r="T58" s="18">
+        <v>2945</v>
+      </c>
+      <c r="U58" s="19">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="59" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I59" s="8" t="s">
         <v>14</v>
       </c>
@@ -2455,8 +2854,17 @@
       <c r="M59" s="9"/>
       <c r="N59" s="9"/>
       <c r="O59" s="9"/>
-    </row>
-    <row r="60" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q59" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="R59" s="9"/>
+      <c r="S59" s="9"/>
+      <c r="T59" s="9"/>
+      <c r="U59" s="9"/>
+      <c r="V59" s="9"/>
+      <c r="W59" s="9"/>
+    </row>
+    <row r="60" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J60" s="1" t="s">
         <v>1</v>
       </c>
@@ -2475,8 +2883,26 @@
       <c r="O60" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="R60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S60" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W60" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I61" t="s">
         <v>5</v>
       </c>
@@ -2499,8 +2925,29 @@
         <v>0</v>
       </c>
       <c r="P61"/>
-    </row>
-    <row r="62" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q61" t="s">
+        <v>5</v>
+      </c>
+      <c r="R61">
+        <v>0.43375961408538199</v>
+      </c>
+      <c r="S61">
+        <v>2.6626381215469599</v>
+      </c>
+      <c r="T61">
+        <v>0.15472473468577</v>
+      </c>
+      <c r="U61">
+        <v>80.697513812154696</v>
+      </c>
+      <c r="V61">
+        <v>0</v>
+      </c>
+      <c r="W61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I62" t="s">
         <v>6</v>
       </c>
@@ -2523,8 +2970,29 @@
         <v>0</v>
       </c>
       <c r="P62"/>
-    </row>
-    <row r="63" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q62" t="s">
+        <v>6</v>
+      </c>
+      <c r="R62">
+        <v>0.42087840697773399</v>
+      </c>
+      <c r="S62">
+        <v>2.6709254143646399</v>
+      </c>
+      <c r="T62">
+        <v>0.227790248454214</v>
+      </c>
+      <c r="U62">
+        <v>81.802486187845304</v>
+      </c>
+      <c r="V62">
+        <v>0</v>
+      </c>
+      <c r="W62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I63" t="s">
         <v>7</v>
       </c>
@@ -2547,8 +3015,29 @@
         <v>0</v>
       </c>
       <c r="P63"/>
-    </row>
-    <row r="64" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q63" t="s">
+        <v>7</v>
+      </c>
+      <c r="R63">
+        <v>0.42668061079856101</v>
+      </c>
+      <c r="S63">
+        <v>2.4979281767955799</v>
+      </c>
+      <c r="T63">
+        <v>0.17905613544910301</v>
+      </c>
+      <c r="U63">
+        <v>81.146408839778999</v>
+      </c>
+      <c r="V63">
+        <v>0</v>
+      </c>
+      <c r="W63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I64" t="s">
         <v>8</v>
       </c>
@@ -2571,8 +3060,29 @@
         <v>0</v>
       </c>
       <c r="P64"/>
-    </row>
-    <row r="65" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q64" t="s">
+        <v>8</v>
+      </c>
+      <c r="R64">
+        <v>0.42612954135039399</v>
+      </c>
+      <c r="S64">
+        <v>2.5379834254143598</v>
+      </c>
+      <c r="T64">
+        <v>0.197789577788194</v>
+      </c>
+      <c r="U64">
+        <v>80.939226519336998</v>
+      </c>
+      <c r="V64">
+        <v>0</v>
+      </c>
+      <c r="W64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I65" t="s">
         <v>9</v>
       </c>
@@ -2595,8 +3105,29 @@
         <v>0</v>
       </c>
       <c r="P65"/>
-    </row>
-    <row r="67" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="Q65" t="s">
+        <v>9</v>
+      </c>
+      <c r="R65">
+        <v>0.42806510054291502</v>
+      </c>
+      <c r="S65">
+        <v>3.2593232044198901</v>
+      </c>
+      <c r="T65">
+        <v>0.19715208765120501</v>
+      </c>
+      <c r="U65">
+        <v>81.077348066298299</v>
+      </c>
+      <c r="V65">
+        <v>0</v>
+      </c>
+      <c r="W65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I67" s="2" t="s">
         <v>10</v>
       </c>
@@ -2616,6 +3147,27 @@
         <v>0</v>
       </c>
       <c r="O67" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R67" s="2">
+        <v>0.42710265475099701</v>
+      </c>
+      <c r="S67" s="2">
+        <v>2.7257596685082799</v>
+      </c>
+      <c r="T67" s="2">
+        <v>0.19130255680569699</v>
+      </c>
+      <c r="U67" s="14">
+        <v>81.132596685082802</v>
+      </c>
+      <c r="V67" s="2">
+        <v>0</v>
+      </c>
+      <c r="W67" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>